<commit_message>
Falta en llenado de campos
</commit_message>
<xml_diff>
--- a/ProyectoparqueaderoPS2025/BDProyectoParqueadero_PS2025.xlsx
+++ b/ProyectoparqueaderoPS2025/BDProyectoParqueadero_PS2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Desktop\ProyectosProgSoft\ProyectoparqueaderoPS2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,11 +478,12 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -558,7 +559,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -596,7 +597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -634,7 +635,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -672,7 +673,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -710,7 +711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -748,7 +749,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -786,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -824,68 +825,233 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>